<commit_message>
add comparison to whisper and glossy, add latency images captured on sat
</commit_message>
<xml_diff>
--- a/results/energy-analysis/energy-consumption.xlsx
+++ b/results/energy-analysis/energy-consumption.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Desktop/VM/jacdac-ota/microbit-samples/results/energy-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F205BD6-7B61-484C-ABB5-4E41E0D23D47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67639286-F2EA-B149-A8D2-1F4E02DED661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{30CE4A45-ABCB-A74E-87BA-8D74890818CE}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{30CE4A45-ABCB-A74E-87BA-8D74890818CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>Number of devices</t>
   </si>
@@ -96,6 +97,45 @@
   </si>
   <si>
     <t>CONNECTED + IDLE</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>Whisper (ms)</t>
+  </si>
+  <si>
+    <t>Glossy (ms)</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>active (ms)</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>battery capacity (mAh)</t>
+  </si>
+  <si>
+    <t>mAh</t>
+  </si>
+  <si>
+    <t>Ron time Whisper</t>
+  </si>
+  <si>
+    <t>Formula is: (Packet size * 8) x TTL + 500</t>
+  </si>
+  <si>
+    <t>(I suspect actual is 2.1</t>
+  </si>
+  <si>
+    <t>I suspect actual is 4.1</t>
   </si>
 </sst>
 </file>
@@ -131,8 +171,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1516,8 +1557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22C6116-72B2-114B-ADC4-0691EDF344F1}">
   <dimension ref="B3:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2155,31 +2196,31 @@
         <v>10</v>
       </c>
       <c r="C31">
-        <v>4.0999999999999996</v>
+        <v>4</v>
       </c>
       <c r="D31">
         <f t="shared" ref="D31:D33" si="14">$O$5/C31</f>
-        <v>487.80487804878055</v>
+        <v>500</v>
       </c>
       <c r="E31">
         <f t="shared" ref="E31:E33" si="15">$O$6/C31</f>
-        <v>548.78048780487813</v>
+        <v>562.5</v>
       </c>
       <c r="F31">
         <f t="shared" ref="F31:F33" si="16">$O$7/C31</f>
-        <v>609.75609756097572</v>
+        <v>625</v>
       </c>
       <c r="G31">
         <f t="shared" ref="G31:G33" si="17">D31/24</f>
-        <v>20.325203252032523</v>
+        <v>20.833333333333332</v>
       </c>
       <c r="H31">
         <f t="shared" ref="H31:H33" si="18">E31/24</f>
-        <v>22.86585365853659</v>
+        <v>23.4375</v>
       </c>
       <c r="I31">
         <f t="shared" ref="I31:I33" si="19">F31/24</f>
-        <v>25.406504065040654</v>
+        <v>26.041666666666668</v>
       </c>
     </row>
     <row r="32" spans="2:12">
@@ -2282,4 +2323,216 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9A147B-64C6-3046-AB41-3BA1FCCCB232}">
+  <dimension ref="A3:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="75.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>1.9</v>
+      </c>
+      <c r="D4">
+        <v>2193</v>
+      </c>
+      <c r="E4">
+        <f>D4*24</f>
+        <v>52632</v>
+      </c>
+      <c r="F4">
+        <v>2000</v>
+      </c>
+      <c r="G4">
+        <f>2000/(B4*(2/3600000))</f>
+        <v>180000000.00000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>3.7</v>
+      </c>
+      <c r="D5">
+        <v>1126</v>
+      </c>
+      <c r="E5">
+        <f>D5*24</f>
+        <v>27024</v>
+      </c>
+      <c r="F5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>1.9</v>
+      </c>
+      <c r="D7">
+        <v>52632</v>
+      </c>
+      <c r="E7">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8" s="1">
+        <f>20 *(2/3600000)</f>
+        <v>1.111111111111111E-5</v>
+      </c>
+      <c r="C8">
+        <f>2000/B8</f>
+        <v>180000000.00000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="F9">
+        <f>2*360000</f>
+        <v>720000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="E11">
+        <f>C4</f>
+        <v>1.9</v>
+      </c>
+      <c r="F11">
+        <f>((E11/1000)*360)</f>
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="G11">
+        <f>ROUND(F11/20,3)</f>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="H11">
+        <f>2000/G11</f>
+        <v>58823.529411764699</v>
+      </c>
+      <c r="I11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="E12">
+        <f>C5</f>
+        <v>3.7</v>
+      </c>
+      <c r="F12">
+        <v>0.76</v>
+      </c>
+      <c r="G12">
+        <f>F12/20</f>
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="H12">
+        <f>2000/G12</f>
+        <v>52631.57894736842</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="E13">
+        <f>C5</f>
+        <v>3.7</v>
+      </c>
+      <c r="F13">
+        <f>((E13/1000)*360)</f>
+        <v>1.3320000000000001</v>
+      </c>
+      <c r="G13">
+        <f>ROUND(F13/20,3)</f>
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H13">
+        <f>2000/G13</f>
+        <v>29850.746268656716</v>
+      </c>
+      <c r="I13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="E14">
+        <v>1.2</v>
+      </c>
+      <c r="F14">
+        <f>((E14/1000)*360)</f>
+        <v>0.43199999999999994</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G13:G14" si="0">F14/20</f>
+        <v>2.1599999999999998E-2</v>
+      </c>
+      <c r="H14">
+        <f>2000/G14</f>
+        <v>92592.592592592599</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add separate scripts for visualising signals
</commit_message>
<xml_diff>
--- a/results/energy-analysis/energy-consumption.xlsx
+++ b/results/energy-analysis/energy-consumption.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Desktop/VM/jacdac-ota/microbit-samples/results/energy-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67639286-F2EA-B149-A8D2-1F4E02DED661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5607BB3-B4C8-3D42-BCD6-93E93B03E249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" activeTab="1" xr2:uid="{30CE4A45-ABCB-A74E-87BA-8D74890818CE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>Number of devices</t>
   </si>
@@ -136,13 +136,22 @@
   </si>
   <si>
     <t>I suspect actual is 4.1</t>
+  </si>
+  <si>
+    <t>RipTide</t>
+  </si>
+  <si>
+    <t>Whisper</t>
+  </si>
+  <si>
+    <t>Glossy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1557,17 +1566,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22C6116-72B2-114B-ADC4-0691EDF344F1}">
   <dimension ref="B3:O34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -1581,7 +1590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1619,7 +1628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>1</v>
       </c>
@@ -1667,7 +1676,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>2</v>
       </c>
@@ -1715,7 +1724,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>3</v>
       </c>
@@ -1763,7 +1772,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>4</v>
       </c>
@@ -1805,7 +1814,7 @@
         <v>12.505002000800319</v>
       </c>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>5</v>
       </c>
@@ -1847,7 +1856,7 @@
         <v>11.599851521900518</v>
       </c>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>6</v>
       </c>
@@ -1858,7 +1867,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -1893,7 +1902,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>1</v>
       </c>
@@ -1935,7 +1944,7 @@
         <v>24.168600154679037</v>
       </c>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>2</v>
       </c>
@@ -1977,7 +1986,7 @@
         <v>24.567610062893081</v>
       </c>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>3</v>
       </c>
@@ -2019,7 +2028,7 @@
         <v>22.305496074232693</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>4</v>
       </c>
@@ -2061,7 +2070,7 @@
         <v>21.792189679218968</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>5</v>
       </c>
@@ -2103,32 +2112,32 @@
         <v>20.5456936226167</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>18</v>
       </c>
@@ -2136,7 +2145,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="2:12">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>7</v>
       </c>
@@ -2159,7 +2168,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>9</v>
       </c>
@@ -2191,7 +2200,7 @@
         <v>28.153153153153152</v>
       </c>
     </row>
-    <row r="31" spans="2:12">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>10</v>
       </c>
@@ -2199,31 +2208,31 @@
         <v>4</v>
       </c>
       <c r="D31">
-        <f t="shared" ref="D31:D33" si="14">$O$5/C31</f>
+        <f t="shared" ref="D31:D32" si="14">$O$5/C31</f>
         <v>500</v>
       </c>
       <c r="E31">
-        <f t="shared" ref="E31:E33" si="15">$O$6/C31</f>
+        <f t="shared" ref="E31:E32" si="15">$O$6/C31</f>
         <v>562.5</v>
       </c>
       <c r="F31">
-        <f t="shared" ref="F31:F33" si="16">$O$7/C31</f>
+        <f t="shared" ref="F31" si="16">$O$7/C31</f>
         <v>625</v>
       </c>
       <c r="G31">
-        <f t="shared" ref="G31:G33" si="17">D31/24</f>
+        <f t="shared" ref="G31" si="17">D31/24</f>
         <v>20.833333333333332</v>
       </c>
       <c r="H31">
-        <f t="shared" ref="H31:H33" si="18">E31/24</f>
+        <f t="shared" ref="H31" si="18">E31/24</f>
         <v>23.4375</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I31:I33" si="19">F31/24</f>
+        <f t="shared" ref="I31" si="19">F31/24</f>
         <v>26.041666666666668</v>
       </c>
     </row>
-    <row r="32" spans="2:12">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>20</v>
       </c>
@@ -2255,7 +2264,7 @@
         <v>32.552083333333336</v>
       </c>
     </row>
-    <row r="33" spans="2:9">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>19</v>
       </c>
@@ -2275,19 +2284,19 @@
         <v>714.28571428571433</v>
       </c>
       <c r="G33">
-        <f>D33/24</f>
+        <f t="shared" ref="G33:I34" si="24">D33/24</f>
         <v>23.80952380952381</v>
       </c>
       <c r="H33">
-        <f>E33/24</f>
+        <f t="shared" si="24"/>
         <v>26.785714285714288</v>
       </c>
       <c r="I33">
-        <f>F33/24</f>
+        <f t="shared" si="24"/>
         <v>29.761904761904763</v>
       </c>
     </row>
-    <row r="34" spans="2:9">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>11</v>
       </c>
@@ -2307,15 +2316,15 @@
         <v>641.02564102564099</v>
       </c>
       <c r="G34">
-        <f>D34/24</f>
+        <f t="shared" si="24"/>
         <v>21.367521367521366</v>
       </c>
       <c r="H34">
-        <f>E34/24</f>
+        <f t="shared" si="24"/>
         <v>24.038461538461537</v>
       </c>
       <c r="I34">
-        <f>F34/24</f>
+        <f t="shared" si="24"/>
         <v>26.709401709401707</v>
       </c>
     </row>
@@ -2329,11 +2338,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD9A147B-64C6-3046-AB41-3BA1FCCCB232}">
   <dimension ref="A3:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="75.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -2342,7 +2351,7 @@
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>21</v>
       </c>
@@ -2359,7 +2368,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2384,7 +2393,7 @@
         <v>180000000.00000003</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2405,7 +2414,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>24</v>
       </c>
@@ -2413,7 +2422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>20</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <f>20 *(2/3600000)</f>
         <v>1.111111111111111E-5</v>
@@ -2437,13 +2446,13 @@
         <v>180000000.00000003</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F9">
         <f>2*360000</f>
         <v>720000</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F10" t="s">
         <v>30</v>
       </c>
@@ -2451,7 +2460,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
       <c r="E11">
         <f>C4</f>
         <v>1.9</v>
@@ -2472,7 +2484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E12">
         <f>C5</f>
         <v>3.7</v>
@@ -2489,7 +2501,10 @@
         <v>52631.57894736842</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
       <c r="E13">
         <f>C5</f>
         <v>3.7</v>
@@ -2510,7 +2525,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
       <c r="E14">
         <v>1.2</v>
       </c>
@@ -2519,7 +2537,7 @@
         <v>0.43199999999999994</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G13:G14" si="0">F14/20</f>
+        <f t="shared" ref="G14" si="0">F14/20</f>
         <v>2.1599999999999998E-2</v>
       </c>
       <c r="H14">
@@ -2527,7 +2545,7 @@
         <v>92592.592592592599</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>31</v>
       </c>

</xml_diff>